<commit_message>
Updated code on timestamp:   03-11-2021 - 15:43:00.80
</commit_message>
<xml_diff>
--- a/level2.xlsx
+++ b/level2.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
+  <workbookPr filterPrivacy="1"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C370D2DD-3D1B-480F-BB67-33EB018971FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="recursion-and-backtracking" sheetId="1" r:id="rId1"/>
@@ -1218,7 +1219,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1542,7 +1543,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:B48"/>
   <sheetViews>
     <sheetView topLeftCell="A19" workbookViewId="0">
@@ -1932,52 +1933,52 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/abbreviation-suing-backtracking-official/ojquestion"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/nqueens-branch-and-bound-official/ojquestion"/>
-    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/max-score-official/ojquestion"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/josephus-problem-official/ojquestion"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/lexicographical-numbers-official/ojquestion"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/gold-mine-2-official/ojquestion"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/solve-sudoku-official/ojquestion"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/crossword-puzzle-official/ojquestion"/>
-    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/cryptarithmetic-official/ojquestion"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/magnets-official/ojquestion"/>
-    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/friends-pairing-2-official/ojquestion"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/k-partitions-official/ojquestion"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/all-palindromic-permutations-official/ojquestion"/>
-    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/all-palindromic-partitions-official/ojquestion"/>
-    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/k-subsets-with-equal-sum-official/ojquestion"/>
-    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/tug-of-war-official/ojquestion"/>
-    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/pattern-matching-official/ojquestion"/>
-    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/wordbreak1official/ojquestion"/>
-    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/remove-invalid-parenthesis-official/ojquestion"/>
-    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/largest-number-at-most-k-swaps-official/ojquestion"/>
-    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/permutation-i-official/ojquestion"/>
-    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/combinations-i-official/ojquestion"/>
-    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/permutations-ii-official/ojquestion"/>
-    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/combinations-2-official/ojquestion"/>
-    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/queens-combinations-2das2d-box-chooses-official/ojquestion"/>
-    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/queens-permutations-2das2d-queen-chooses-official/ojquestion"/>
-    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/queens-permutations-2das2d-box-chooses-official/ojquestion"/>
-    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/queens-combinations-2das2d-official/ojquestion"/>
-    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/queens-combinations-2das1d-queen-chooses-official/ojquestion"/>
-    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/nqueens-combinations-2das1d-queen-chooses-official/ojquestion"/>
-    <hyperlink ref="B33" r:id="rId31" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/nknights-combinations-2das1d-knight-chooses-official/ojquestion"/>
-    <hyperlink ref="B34" r:id="rId32" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/nqueens-permutations-2das1d-official-queen-chooses/ojquestion"/>
-    <hyperlink ref="B35" r:id="rId33" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/permutations-words-1-official/ojquestion"/>
-    <hyperlink ref="B36" r:id="rId34" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/permutations-words-2-official/ojquestion"/>
-    <hyperlink ref="B37" r:id="rId35" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/words-kselection-1-official/ojquestion"/>
-    <hyperlink ref="B38" r:id="rId36" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/word-kselection-2-official/ojquestion"/>
-    <hyperlink ref="B39" r:id="rId37" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/words-klength-words-1-official/ojquestion"/>
-    <hyperlink ref="B40" r:id="rId38" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/words-klength-words-2-official/ojquestion"/>
-    <hyperlink ref="B41" r:id="rId39" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/words-kselection-3-official/ojquestion"/>
-    <hyperlink ref="B42" r:id="rId40" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/words-kselection-4-official/ojquestion"/>
-    <hyperlink ref="B43" r:id="rId41" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/wors-klength-words-3-official/ojquestion"/>
-    <hyperlink ref="B44" r:id="rId42" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/words-klength-words-4-official/ojquestion"/>
-    <hyperlink ref="B45" r:id="rId43" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/coin-change-combinations-1-official/ojquestion"/>
-    <hyperlink ref="B46" r:id="rId44" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/coin-change-combinations-2-official/ojquestion"/>
-    <hyperlink ref="B47" r:id="rId45" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/coin-change-permutations-1-official/ojquestion"/>
-    <hyperlink ref="B48" r:id="rId46" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/coin-change-permutations-2-official/ojquestion"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/abbreviation-suing-backtracking-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/nqueens-branch-and-bound-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/max-score-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/josephus-problem-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/lexicographical-numbers-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/gold-mine-2-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/solve-sudoku-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/crossword-puzzle-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/cryptarithmetic-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000008000000}"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/magnets-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000009000000}"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/friends-pairing-2-official/ojquestion" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/k-partitions-official/ojquestion" xr:uid="{00000000-0004-0000-0000-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/all-palindromic-permutations-official/ojquestion" xr:uid="{00000000-0004-0000-0000-00000C000000}"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/all-palindromic-partitions-official/ojquestion" xr:uid="{00000000-0004-0000-0000-00000D000000}"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/k-subsets-with-equal-sum-official/ojquestion" xr:uid="{00000000-0004-0000-0000-00000E000000}"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/tug-of-war-official/ojquestion" xr:uid="{00000000-0004-0000-0000-00000F000000}"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/pattern-matching-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000010000000}"/>
+    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/wordbreak1official/ojquestion" xr:uid="{00000000-0004-0000-0000-000011000000}"/>
+    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/remove-invalid-parenthesis-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000012000000}"/>
+    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/largest-number-at-most-k-swaps-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000013000000}"/>
+    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/permutation-i-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000014000000}"/>
+    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/combinations-i-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000015000000}"/>
+    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/permutations-ii-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000016000000}"/>
+    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/combinations-2-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000017000000}"/>
+    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/queens-combinations-2das2d-box-chooses-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000018000000}"/>
+    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/queens-permutations-2das2d-queen-chooses-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000019000000}"/>
+    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/queens-permutations-2das2d-box-chooses-official/ojquestion" xr:uid="{00000000-0004-0000-0000-00001A000000}"/>
+    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/queens-combinations-2das2d-official/ojquestion" xr:uid="{00000000-0004-0000-0000-00001B000000}"/>
+    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/queens-combinations-2das1d-queen-chooses-official/ojquestion" xr:uid="{00000000-0004-0000-0000-00001C000000}"/>
+    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/nqueens-combinations-2das1d-queen-chooses-official/ojquestion" xr:uid="{00000000-0004-0000-0000-00001D000000}"/>
+    <hyperlink ref="B33" r:id="rId31" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/nknights-combinations-2das1d-knight-chooses-official/ojquestion" xr:uid="{00000000-0004-0000-0000-00001E000000}"/>
+    <hyperlink ref="B34" r:id="rId32" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/nqueens-permutations-2das1d-official-queen-chooses/ojquestion" xr:uid="{00000000-0004-0000-0000-00001F000000}"/>
+    <hyperlink ref="B35" r:id="rId33" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/permutations-words-1-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000020000000}"/>
+    <hyperlink ref="B36" r:id="rId34" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/permutations-words-2-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000021000000}"/>
+    <hyperlink ref="B37" r:id="rId35" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/words-kselection-1-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000022000000}"/>
+    <hyperlink ref="B38" r:id="rId36" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/word-kselection-2-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000023000000}"/>
+    <hyperlink ref="B39" r:id="rId37" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/words-klength-words-1-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000024000000}"/>
+    <hyperlink ref="B40" r:id="rId38" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/words-klength-words-2-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000025000000}"/>
+    <hyperlink ref="B41" r:id="rId39" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/words-kselection-3-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000026000000}"/>
+    <hyperlink ref="B42" r:id="rId40" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/words-kselection-4-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000027000000}"/>
+    <hyperlink ref="B43" r:id="rId41" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/wors-klength-words-3-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000028000000}"/>
+    <hyperlink ref="B44" r:id="rId42" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/words-klength-words-4-official/ojquestion" xr:uid="{00000000-0004-0000-0000-000029000000}"/>
+    <hyperlink ref="B45" r:id="rId43" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/coin-change-combinations-1-official/ojquestion" xr:uid="{00000000-0004-0000-0000-00002A000000}"/>
+    <hyperlink ref="B46" r:id="rId44" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/coin-change-combinations-2-official/ojquestion" xr:uid="{00000000-0004-0000-0000-00002B000000}"/>
+    <hyperlink ref="B47" r:id="rId45" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/coin-change-permutations-1-official/ojquestion" xr:uid="{00000000-0004-0000-0000-00002C000000}"/>
+    <hyperlink ref="B48" r:id="rId46" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/recursion-and-backtracking/coin-change-permutations-2-official/ojquestion" xr:uid="{00000000-0004-0000-0000-00002D000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId47"/>
@@ -1985,11 +1986,11 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+  <dimension ref="A2:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A36"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2277,49 +2278,54 @@
         <v>394</v>
       </c>
     </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>35</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/marks_of_pcm/ojquestion"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/union_of_two_sorted_arrays/ojquestion"/>
-    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/search_a_2d_matrix/ojquestion"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/search_a_2d_matrix_ii/ojquestion"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/find_pivot_index/ojquestion"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/find_k_closest_elements/ojquestion"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/find_pair_with_given_difference/ojquestion"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/roof_top/ojquestion"/>
-    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/maximize_sum_of_arr%5bi%5d*i_of_an_array/ojquestion"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/count_inversions/ojquestion"/>
-    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/find-first-and-last-postion-of-element-in-sorted-array/ojquestion"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/max-sum-in-the-configuration/ojquestion"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/search_in_rotated_sorted_array/ojquestion"/>
-    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/find_minimum_in_rotated_sorted_array/ojquestion"/>
-    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/find_rotation_count/ojquestion"/>
-    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/median-of-two-sorted-arrays/ojquestion"/>
-    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/koko_eating_bananas/ojquestion"/>
-    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/find-the-smallest-divisor-given-a-threshold/ojquestion"/>
-    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/chocolate-distribution/ojquestion"/>
-    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/allocate_minimum_number_of_pages/ojquestion"/>
-    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/split_array_largest_sum/ojquestion"/>
-    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/capacity_to_ship_within_d_days/ojquestion"/>
-    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/count-the-triplets-official/ojquestion"/>
-    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/count-possible-triangles-official/ojquestion"/>
-    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/count-zeros-in-a-sorted-matrix-official/ojquestion"/>
-    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/counting-elements-in-two-arrays-official/ojquestion"/>
-    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/count-zeros-xor-pairs-official/ojquestion"/>
-    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/facing-the-sun-official/ojquestion"/>
-    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/distinct-absolute-array-elements-official/ojquestion"/>
-    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/find-transition-point-official/ojquestion"/>
-    <hyperlink ref="B33" r:id="rId31" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/first-bad-version-official/ojquestion"/>
-    <hyperlink ref="B34" r:id="rId32" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/guess-number-higher-or-lower-official/ojquestion"/>
-    <hyperlink ref="B35" r:id="rId33" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/find-the-element-that-appears-once-in-sorted-array--offcial/ojquestion"/>
-    <hyperlink ref="B36" r:id="rId34" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/maximum-number-of-1s-row-official/ojquestion"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/marks_of_pcm/ojquestion" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/union_of_two_sorted_arrays/ojquestion" xr:uid="{00000000-0004-0000-0900-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/search_a_2d_matrix/ojquestion" xr:uid="{00000000-0004-0000-0900-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/search_a_2d_matrix_ii/ojquestion" xr:uid="{00000000-0004-0000-0900-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/find_pivot_index/ojquestion" xr:uid="{00000000-0004-0000-0900-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/find_k_closest_elements/ojquestion" xr:uid="{00000000-0004-0000-0900-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/find_pair_with_given_difference/ojquestion" xr:uid="{00000000-0004-0000-0900-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/roof_top/ojquestion" xr:uid="{00000000-0004-0000-0900-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/maximize_sum_of_arr%5bi%5d*i_of_an_array/ojquestion" xr:uid="{00000000-0004-0000-0900-000008000000}"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/count_inversions/ojquestion" xr:uid="{00000000-0004-0000-0900-000009000000}"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/find-first-and-last-postion-of-element-in-sorted-array/ojquestion" xr:uid="{00000000-0004-0000-0900-00000A000000}"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/max-sum-in-the-configuration/ojquestion" xr:uid="{00000000-0004-0000-0900-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/search_in_rotated_sorted_array/ojquestion" xr:uid="{00000000-0004-0000-0900-00000C000000}"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/find_minimum_in_rotated_sorted_array/ojquestion" xr:uid="{00000000-0004-0000-0900-00000D000000}"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/find_rotation_count/ojquestion" xr:uid="{00000000-0004-0000-0900-00000E000000}"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/median-of-two-sorted-arrays/ojquestion" xr:uid="{00000000-0004-0000-0900-00000F000000}"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/koko_eating_bananas/ojquestion" xr:uid="{00000000-0004-0000-0900-000010000000}"/>
+    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/find-the-smallest-divisor-given-a-threshold/ojquestion" xr:uid="{00000000-0004-0000-0900-000011000000}"/>
+    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/chocolate-distribution/ojquestion" xr:uid="{00000000-0004-0000-0900-000012000000}"/>
+    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/allocate_minimum_number_of_pages/ojquestion" xr:uid="{00000000-0004-0000-0900-000013000000}"/>
+    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/split_array_largest_sum/ojquestion" xr:uid="{00000000-0004-0000-0900-000014000000}"/>
+    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/capacity_to_ship_within_d_days/ojquestion" xr:uid="{00000000-0004-0000-0900-000015000000}"/>
+    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/count-the-triplets-official/ojquestion" xr:uid="{00000000-0004-0000-0900-000016000000}"/>
+    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/count-possible-triangles-official/ojquestion" xr:uid="{00000000-0004-0000-0900-000017000000}"/>
+    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/count-zeros-in-a-sorted-matrix-official/ojquestion" xr:uid="{00000000-0004-0000-0900-000018000000}"/>
+    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/counting-elements-in-two-arrays-official/ojquestion" xr:uid="{00000000-0004-0000-0900-000019000000}"/>
+    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/count-zeros-xor-pairs-official/ojquestion" xr:uid="{00000000-0004-0000-0900-00001A000000}"/>
+    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/facing-the-sun-official/ojquestion" xr:uid="{00000000-0004-0000-0900-00001B000000}"/>
+    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/distinct-absolute-array-elements-official/ojquestion" xr:uid="{00000000-0004-0000-0900-00001C000000}"/>
+    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/find-transition-point-official/ojquestion" xr:uid="{00000000-0004-0000-0900-00001D000000}"/>
+    <hyperlink ref="B33" r:id="rId31" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/first-bad-version-official/ojquestion" xr:uid="{00000000-0004-0000-0900-00001E000000}"/>
+    <hyperlink ref="B34" r:id="rId32" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/guess-number-higher-or-lower-official/ojquestion" xr:uid="{00000000-0004-0000-0900-00001F000000}"/>
+    <hyperlink ref="B35" r:id="rId33" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/find-the-element-that-appears-once-in-sorted-array--offcial/ojquestion" xr:uid="{00000000-0004-0000-0900-000020000000}"/>
+    <hyperlink ref="B36" r:id="rId34" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/searching-and-sorting/maximum-number-of-1s-row-official/ojquestion" xr:uid="{00000000-0004-0000-0900-000021000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2581,43 +2587,43 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/basics-of-bit-official/ojquestion"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/print-value-of-rsb-mask-official/ojquestion"/>
-    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/kernighans-algo-official/ojquestion"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/josephus-special-official/ojquestion"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/gray-code/ojquestion"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/minimum-number-of-software-developers-official/ojquestion"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/number-of-valid-words-official/ojquestion"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/all-repeating-except-one-official/ojquestion"/>
-    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/all-repeating-except-two-official/ojquestion"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/one-repeating-and-one-missing-official/ojquestion"/>
-    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/all-repeating-three-times-except-one-official/ojquestion"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/triplets-1-official/ojquestion"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/reduce-n-to-1-official/ojquestion"/>
-    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/pepcoder-and-bits-official/ojquestion"/>
-    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/xor-sum-pair-official/ojquestion"/>
-    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/abrreviation1-using-bits-official/ojquestion"/>
-    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/utf-8-encoding-official/ojquestion"/>
-    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/sudoku-using-bit-manipulation-official/ojquestion"/>
-    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/nqueens-using-bits-official/ojquestion"/>
-    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/flip-bits-to-convert-a-to-b-official/ojquestion"/>
-    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/copy-set-bits-in-a-range-official/ojquestion"/>
-    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/is-a-power-of-2-official/ojquestion"/>
-    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/solve-7nby8-official/ojquestion"/>
-    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/swap-all-odd-and-even-bits-official/ojquestion"/>
-    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/sum-of-bit-differences-of-all-pairs-official/ojquestion"/>
-    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/check-divisibility-by-3-official/ojquestion"/>
-    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/count-setbits-in-first-n-natural-numbers-official/ojquestion"/>
-    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/print-binary-and-reverse-bits-official/ojquestion"/>
-    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/min-xor-pairs-official/ojquestion"/>
-    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/nth-palindromic-binary-official/ojquestion"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/basics-of-bit-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/print-value-of-rsb-mask-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/kernighans-algo-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/josephus-special-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/gray-code/ojquestion" xr:uid="{00000000-0004-0000-0100-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/minimum-number-of-software-developers-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/number-of-valid-words-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/all-repeating-except-one-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/all-repeating-except-two-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000008000000}"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/one-repeating-and-one-missing-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000009000000}"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/all-repeating-three-times-except-one-official/ojquestion" xr:uid="{00000000-0004-0000-0100-00000A000000}"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/triplets-1-official/ojquestion" xr:uid="{00000000-0004-0000-0100-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/reduce-n-to-1-official/ojquestion" xr:uid="{00000000-0004-0000-0100-00000C000000}"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/pepcoder-and-bits-official/ojquestion" xr:uid="{00000000-0004-0000-0100-00000D000000}"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/xor-sum-pair-official/ojquestion" xr:uid="{00000000-0004-0000-0100-00000E000000}"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/abrreviation1-using-bits-official/ojquestion" xr:uid="{00000000-0004-0000-0100-00000F000000}"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/utf-8-encoding-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000010000000}"/>
+    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/sudoku-using-bit-manipulation-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000011000000}"/>
+    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/nqueens-using-bits-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000012000000}"/>
+    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/flip-bits-to-convert-a-to-b-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000013000000}"/>
+    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/copy-set-bits-in-a-range-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000014000000}"/>
+    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/is-a-power-of-2-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000015000000}"/>
+    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/solve-7nby8-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000016000000}"/>
+    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/swap-all-odd-and-even-bits-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000017000000}"/>
+    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/sum-of-bit-differences-of-all-pairs-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000018000000}"/>
+    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/check-divisibility-by-3-official/ojquestion" xr:uid="{00000000-0004-0000-0100-000019000000}"/>
+    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/count-setbits-in-first-n-natural-numbers-official/ojquestion" xr:uid="{00000000-0004-0000-0100-00001A000000}"/>
+    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/print-binary-and-reverse-bits-official/ojquestion" xr:uid="{00000000-0004-0000-0100-00001B000000}"/>
+    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/min-xor-pairs-official/ojquestion" xr:uid="{00000000-0004-0000-0100-00001C000000}"/>
+    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/bit-manipulation/nth-palindromic-binary-official/ojquestion" xr:uid="{00000000-0004-0000-0100-00001D000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A2:B83"/>
   <sheetViews>
     <sheetView topLeftCell="A61" workbookViewId="0">
@@ -3287,94 +3293,94 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/lis-official/ojquestion"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/msis-official/ojquestion"/>
-    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/lbs-official/ojquestion"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/max-non-overlapping-bridges-official/ojquestion"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/russian-doll-envelopes-official/ojquestion"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/min-squares-official/ojquestion"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/lcs-official/ojquestion"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/lps-official/ojquestion"/>
-    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/cps-official/ojquestion"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/cpss-official/ojquestion"/>
-    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/lpss-official/ojquestion"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/count-distinct-subsequences-official/ojquestion"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/count-of-distinct-palindromic-subsequences-official/ojquestion"/>
-    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/lis-re-official/ojquestion"/>
-    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/min-jumps-re-official/ojquestion"/>
-    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/minimum-cost-path-re-official/ojquestion"/>
-    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/goldmine-re-official/ojquestion"/>
-    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/print-all-paths-with-target-sum-subset-official/ojquestion"/>
-    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/zero-one-knapsack-re-official/ojquestion"/>
-    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/wildcard-pattern-matching-official/ojquestion"/>
-    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/regular-expression-matching-official/ojquestion"/>
-    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/catalan-number-official/ojquestion"/>
-    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/count-bst-official/ojquestion"/>
-    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/count-valleys-mountains-official/ojquestion"/>
-    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/count-brackets-official/ojquestion"/>
-    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/circle-and-chords-official/ojquestion"/>
-    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/number-of-ways-of-triangulation-official/ojquestion"/>
-    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/minimum-score-of-triangulation-official/ojquestion"/>
-    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/cn-variations/video"/>
-    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/rod-cutting-official/ojquestion"/>
-    <hyperlink ref="B33" r:id="rId31" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/min-palindromic-cut-official/ojquestion"/>
-    <hyperlink ref="B34" r:id="rId32" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/matrix-chain-multiplication-official/ojquestion"/>
-    <hyperlink ref="B35" r:id="rId33" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/boolean-parenthesization-official/ojquestion"/>
-    <hyperlink ref="B36" r:id="rId34" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/optimal-bst-official/ojquestion"/>
-    <hyperlink ref="B37" r:id="rId35" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/burst-balloons-official/ojquestion"/>
-    <hyperlink ref="B38" r:id="rId36" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/longest-common-substring-official/ojquestion"/>
-    <hyperlink ref="B39" r:id="rId37" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/longest-repeating-subsequence-official/ojquestion"/>
-    <hyperlink ref="B40" r:id="rId38" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/minimum-ascii-delete-sum-for-two-strings-official/ojquestion"/>
-    <hyperlink ref="B41" r:id="rId39" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/minimum-cost-to-make-two-strings-identical-official/ojquestion"/>
-    <hyperlink ref="B42" r:id="rId40" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/shortest-uncommon-subsequence-official/ojquestion"/>
-    <hyperlink ref="B43" r:id="rId41" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/distinct-transformations-official/ojquestion"/>
-    <hyperlink ref="B44" r:id="rId42" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/probability-of-knight-in-the-chessboard-official/ojquestion"/>
-    <hyperlink ref="B45" r:id="rId43" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/edit-distance-official/ojquestion"/>
-    <hyperlink ref="B46" r:id="rId44" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/kadanes-algorithm-official/ojquestion"/>
-    <hyperlink ref="B47" r:id="rId45" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/k-concatenation-official/ojquestion"/>
-    <hyperlink ref="B48" r:id="rId46" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/maximum-sum-subarray-with-at-least-k-elements-official/ojquestion"/>
-    <hyperlink ref="B49" r:id="rId47" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/numeric-keypad-official/ojquestion"/>
-    <hyperlink ref="B50" r:id="rId48" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/maximum-difference-of-zeros-and-ones-in-binary-string-official/ojquestion"/>
-    <hyperlink ref="B51" r:id="rId49" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/maximum-sum-of-two-non-overlapping-subarrays-official/ojquestion"/>
-    <hyperlink ref="B52" r:id="rId50" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/optimal-strategy-for-a-game-official/ojquestion"/>
-    <hyperlink ref="B53" r:id="rId51" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/egg-drop-official/ojquestion"/>
-    <hyperlink ref="B54" r:id="rId52" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/maximum-sum-of-three-non-ovarlapping-subarrays-official/ojquestion"/>
-    <hyperlink ref="B55" r:id="rId53" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/maximum-sum-of-m-non-overlapping-subarrays-official/ojquestion"/>
-    <hyperlink ref="B56" r:id="rId54" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/floor-tiling-2-official/ojquestion"/>
-    <hyperlink ref="B57" r:id="rId55" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/cherry-pickup-official/ojquestion"/>
-    <hyperlink ref="B58" r:id="rId56" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/scramble-string-official/ojquestion"/>
-    <hyperlink ref="B59" r:id="rId57" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/lcs-of-three-strings-official/ojquestion"/>
-    <hyperlink ref="B60" r:id="rId58" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/arithmetic-slices-1-official/ojquestion"/>
-    <hyperlink ref="B61" r:id="rId59" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/arithmetic-slices-2-official/ojquestion"/>
-    <hyperlink ref="B62" r:id="rId60" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/word-break-2-official/ojquestion"/>
-    <hyperlink ref="B63" r:id="rId61" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/wordwrap-official/ojquestion"/>
-    <hyperlink ref="B64" r:id="rId62" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/2-key-keyboard-official/ojquestion"/>
-    <hyperlink ref="B65" r:id="rId63" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/4-key-keyboard-official/ojquestion"/>
-    <hyperlink ref="B66" r:id="rId64" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/largest-square-sub-matrix-with-all-ones-official/ojquestion"/>
-    <hyperlink ref="B67" r:id="rId65" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/highway-billboard-official/ojquestion"/>
-    <hyperlink ref="B68" r:id="rId66" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/temple-offerings-official/ojquestion"/>
-    <hyperlink ref="B69" r:id="rId67" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/alternating-subsequence-with-maximum-sum-official/ojquestion"/>
-    <hyperlink ref="B70" r:id="rId68" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/minimum-insertions-to-make-palindrome-official/ojquestion"/>
-    <hyperlink ref="B71" r:id="rId69" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/minimum-delta-in-partitions-official/ojquestion"/>
-    <hyperlink ref="B72" r:id="rId70" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/minimum-number-of-steps-to-reduce-n-official/ojquestion"/>
-    <hyperlink ref="B73" r:id="rId71" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/minimum-number-of-steps-to-form-n-official/ojquestion"/>
-    <hyperlink ref="B74" r:id="rId72" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/linear-equation-of-n-variables-official/ojquestion"/>
-    <hyperlink ref="B75" r:id="rId73" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/minimum-deletions-to-make-palindromic-sequence-official/ojquestion"/>
-    <hyperlink ref="B76" r:id="rId74" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/minimum-deletions-to-make-sorted-array/ojquestion"/>
-    <hyperlink ref="B77" r:id="rId75" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/min-max-value-expression-official/ojquestion"/>
-    <hyperlink ref="B78" r:id="rId76" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/ugly-number-official/ojquestion"/>
-    <hyperlink ref="B79" r:id="rId77" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/super-ugly-number-official/ojquestion"/>
-    <hyperlink ref="B80" r:id="rId78" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/find-water-in-glass-official/ojquestion"/>
-    <hyperlink ref="B81" r:id="rId79" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/frog-jump-official/ojquestion"/>
-    <hyperlink ref="B82" r:id="rId80" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/interleaving-of-two-strings-official/ojquestion"/>
-    <hyperlink ref="B83" r:id="rId81" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/maximum-length-of-repeated-subarray-official/ojquestion"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/lis-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/msis-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/lbs-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/max-non-overlapping-bridges-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/russian-doll-envelopes-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/min-squares-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/lcs-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/lps-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/cps-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000008000000}"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/cpss-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000009000000}"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/lpss-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00000A000000}"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/count-distinct-subsequences-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/count-of-distinct-palindromic-subsequences-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00000C000000}"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/lis-re-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00000D000000}"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/min-jumps-re-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00000E000000}"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/minimum-cost-path-re-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00000F000000}"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/goldmine-re-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000010000000}"/>
+    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/print-all-paths-with-target-sum-subset-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000011000000}"/>
+    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/zero-one-knapsack-re-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000012000000}"/>
+    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/wildcard-pattern-matching-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000013000000}"/>
+    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/regular-expression-matching-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000014000000}"/>
+    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/catalan-number-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000015000000}"/>
+    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/count-bst-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000016000000}"/>
+    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/count-valleys-mountains-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000017000000}"/>
+    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/count-brackets-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000018000000}"/>
+    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/circle-and-chords-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000019000000}"/>
+    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/number-of-ways-of-triangulation-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00001A000000}"/>
+    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/minimum-score-of-triangulation-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00001B000000}"/>
+    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/cn-variations/video" xr:uid="{00000000-0004-0000-0200-00001C000000}"/>
+    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/rod-cutting-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00001D000000}"/>
+    <hyperlink ref="B33" r:id="rId31" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/min-palindromic-cut-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00001E000000}"/>
+    <hyperlink ref="B34" r:id="rId32" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/matrix-chain-multiplication-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00001F000000}"/>
+    <hyperlink ref="B35" r:id="rId33" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/boolean-parenthesization-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000020000000}"/>
+    <hyperlink ref="B36" r:id="rId34" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/optimal-bst-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000021000000}"/>
+    <hyperlink ref="B37" r:id="rId35" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/burst-balloons-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000022000000}"/>
+    <hyperlink ref="B38" r:id="rId36" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/longest-common-substring-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000023000000}"/>
+    <hyperlink ref="B39" r:id="rId37" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/longest-repeating-subsequence-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000024000000}"/>
+    <hyperlink ref="B40" r:id="rId38" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/minimum-ascii-delete-sum-for-two-strings-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000025000000}"/>
+    <hyperlink ref="B41" r:id="rId39" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/minimum-cost-to-make-two-strings-identical-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000026000000}"/>
+    <hyperlink ref="B42" r:id="rId40" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/shortest-uncommon-subsequence-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000027000000}"/>
+    <hyperlink ref="B43" r:id="rId41" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/distinct-transformations-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000028000000}"/>
+    <hyperlink ref="B44" r:id="rId42" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/probability-of-knight-in-the-chessboard-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000029000000}"/>
+    <hyperlink ref="B45" r:id="rId43" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/edit-distance-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00002A000000}"/>
+    <hyperlink ref="B46" r:id="rId44" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/kadanes-algorithm-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00002B000000}"/>
+    <hyperlink ref="B47" r:id="rId45" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/k-concatenation-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00002C000000}"/>
+    <hyperlink ref="B48" r:id="rId46" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/maximum-sum-subarray-with-at-least-k-elements-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00002D000000}"/>
+    <hyperlink ref="B49" r:id="rId47" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/numeric-keypad-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00002E000000}"/>
+    <hyperlink ref="B50" r:id="rId48" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/maximum-difference-of-zeros-and-ones-in-binary-string-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00002F000000}"/>
+    <hyperlink ref="B51" r:id="rId49" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/maximum-sum-of-two-non-overlapping-subarrays-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000030000000}"/>
+    <hyperlink ref="B52" r:id="rId50" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/optimal-strategy-for-a-game-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000031000000}"/>
+    <hyperlink ref="B53" r:id="rId51" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/egg-drop-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000032000000}"/>
+    <hyperlink ref="B54" r:id="rId52" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/maximum-sum-of-three-non-ovarlapping-subarrays-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000033000000}"/>
+    <hyperlink ref="B55" r:id="rId53" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/maximum-sum-of-m-non-overlapping-subarrays-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000034000000}"/>
+    <hyperlink ref="B56" r:id="rId54" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/floor-tiling-2-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000035000000}"/>
+    <hyperlink ref="B57" r:id="rId55" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/cherry-pickup-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000036000000}"/>
+    <hyperlink ref="B58" r:id="rId56" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/scramble-string-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000037000000}"/>
+    <hyperlink ref="B59" r:id="rId57" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/lcs-of-three-strings-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000038000000}"/>
+    <hyperlink ref="B60" r:id="rId58" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/arithmetic-slices-1-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000039000000}"/>
+    <hyperlink ref="B61" r:id="rId59" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/arithmetic-slices-2-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00003A000000}"/>
+    <hyperlink ref="B62" r:id="rId60" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/word-break-2-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00003B000000}"/>
+    <hyperlink ref="B63" r:id="rId61" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/wordwrap-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00003C000000}"/>
+    <hyperlink ref="B64" r:id="rId62" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/2-key-keyboard-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00003D000000}"/>
+    <hyperlink ref="B65" r:id="rId63" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/4-key-keyboard-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00003E000000}"/>
+    <hyperlink ref="B66" r:id="rId64" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/largest-square-sub-matrix-with-all-ones-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00003F000000}"/>
+    <hyperlink ref="B67" r:id="rId65" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/highway-billboard-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000040000000}"/>
+    <hyperlink ref="B68" r:id="rId66" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/temple-offerings-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000041000000}"/>
+    <hyperlink ref="B69" r:id="rId67" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/alternating-subsequence-with-maximum-sum-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000042000000}"/>
+    <hyperlink ref="B70" r:id="rId68" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/minimum-insertions-to-make-palindrome-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000043000000}"/>
+    <hyperlink ref="B71" r:id="rId69" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/minimum-delta-in-partitions-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000044000000}"/>
+    <hyperlink ref="B72" r:id="rId70" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/minimum-number-of-steps-to-reduce-n-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000045000000}"/>
+    <hyperlink ref="B73" r:id="rId71" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/minimum-number-of-steps-to-form-n-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000046000000}"/>
+    <hyperlink ref="B74" r:id="rId72" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/linear-equation-of-n-variables-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000047000000}"/>
+    <hyperlink ref="B75" r:id="rId73" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/minimum-deletions-to-make-palindromic-sequence-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000048000000}"/>
+    <hyperlink ref="B76" r:id="rId74" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/minimum-deletions-to-make-sorted-array/ojquestion" xr:uid="{00000000-0004-0000-0200-000049000000}"/>
+    <hyperlink ref="B77" r:id="rId75" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/min-max-value-expression-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00004A000000}"/>
+    <hyperlink ref="B78" r:id="rId76" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/ugly-number-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00004B000000}"/>
+    <hyperlink ref="B79" r:id="rId77" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/super-ugly-number-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00004C000000}"/>
+    <hyperlink ref="B80" r:id="rId78" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/find-water-in-glass-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00004D000000}"/>
+    <hyperlink ref="B81" r:id="rId79" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/frog-jump-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00004E000000}"/>
+    <hyperlink ref="B82" r:id="rId80" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/interleaving-of-two-strings-official/ojquestion" xr:uid="{00000000-0004-0000-0200-00004F000000}"/>
+    <hyperlink ref="B83" r:id="rId81" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/dynamic-programming/maximum-length-of-repeated-subarray-official/ojquestion" xr:uid="{00000000-0004-0000-0200-000050000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3652,45 +3658,45 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/cameras-in-binary-tree-official/ojquestion"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/levelup_house-robber-in-binary-tree/ojquestion"/>
-    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/longest-zigzag-path-in-a-binary-tree/ojquestion"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/levelup_validate-bst/ojquestion"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/recover-bst/ojquestion"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-binarytree-from-preorder-and-inorder-traversal/ojquestion"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-binarytree-from-postorder-and-inorder-traversal/ojquestion"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-binary-tree-from-levelorder-and-inorder-traversal/ojquestion"/>
-    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-binarytree-from-preorder-and-postorder-traversal/ojquestion"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-bst-from-inorder-traversal/ojquestion"/>
-    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-bst-from-preorder-traversal/ojquestion"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-bst-from-postorder-traversal/ojquestion"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-bst-from-levelorder-traversal/ojquestion"/>
-    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/serialize-and-deserialize-binary-tree/ojquestion"/>
-    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/left-view-of-a-binarytree/ojquestion"/>
-    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/right-view-of-a-binarytree/ojquestion"/>
-    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/width-of-a-binary-tree/ojquestion"/>
-    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/vertical-order-traversal-of-a-binarytree/ojquestion"/>
-    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/vertical-order-traversal-of-a-binarytree-ii/ojquestion"/>
-    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/bottom-view-of-a-binarytree/ojquestion"/>
-    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/top-view-of-a-binarytree/ojquestion"/>
-    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/diagonal-order-of-a-binarytree/ojquestion"/>
-    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/diagonal-order-(anti-clock-wise)-of-a-binarytree/ojquestion"/>
-    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/vertical-order-sum-of-a-binarytree/ojquestion"/>
-    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/diagonal-order-sum-of-a-binary-tree/ojquestion"/>
-    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/in-order-morris-traversal-in-binarytree/ojquestion"/>
-    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/pre-order-morris-traversal-in-binary-tree/ojquestion"/>
-    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/bst-iterator/ojquestion"/>
-    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/node-to-root-path-binary-tree/ojquestion"/>
-    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/root-to-all-leaf-path-in-binary-tree/ojquestion"/>
-    <hyperlink ref="B33" r:id="rId31" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/all-single-child-parent-in-binary-tree/ojquestion"/>
-    <hyperlink ref="B34" r:id="rId32" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/count-all-single-child-parent-in-binary-tree/ojquestion"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/cameras-in-binary-tree-official/ojquestion" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/levelup_house-robber-in-binary-tree/ojquestion" xr:uid="{00000000-0004-0000-0300-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/longest-zigzag-path-in-a-binary-tree/ojquestion" xr:uid="{00000000-0004-0000-0300-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/levelup_validate-bst/ojquestion" xr:uid="{00000000-0004-0000-0300-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/recover-bst/ojquestion" xr:uid="{00000000-0004-0000-0300-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-binarytree-from-preorder-and-inorder-traversal/ojquestion" xr:uid="{00000000-0004-0000-0300-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-binarytree-from-postorder-and-inorder-traversal/ojquestion" xr:uid="{00000000-0004-0000-0300-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-binary-tree-from-levelorder-and-inorder-traversal/ojquestion" xr:uid="{00000000-0004-0000-0300-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-binarytree-from-preorder-and-postorder-traversal/ojquestion" xr:uid="{00000000-0004-0000-0300-000008000000}"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-bst-from-inorder-traversal/ojquestion" xr:uid="{00000000-0004-0000-0300-000009000000}"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-bst-from-preorder-traversal/ojquestion" xr:uid="{00000000-0004-0000-0300-00000A000000}"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-bst-from-postorder-traversal/ojquestion" xr:uid="{00000000-0004-0000-0300-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/construct-bst-from-levelorder-traversal/ojquestion" xr:uid="{00000000-0004-0000-0300-00000C000000}"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/serialize-and-deserialize-binary-tree/ojquestion" xr:uid="{00000000-0004-0000-0300-00000D000000}"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/left-view-of-a-binarytree/ojquestion" xr:uid="{00000000-0004-0000-0300-00000E000000}"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/right-view-of-a-binarytree/ojquestion" xr:uid="{00000000-0004-0000-0300-00000F000000}"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/width-of-a-binary-tree/ojquestion" xr:uid="{00000000-0004-0000-0300-000010000000}"/>
+    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/vertical-order-traversal-of-a-binarytree/ojquestion" xr:uid="{00000000-0004-0000-0300-000011000000}"/>
+    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/vertical-order-traversal-of-a-binarytree-ii/ojquestion" xr:uid="{00000000-0004-0000-0300-000012000000}"/>
+    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/bottom-view-of-a-binarytree/ojquestion" xr:uid="{00000000-0004-0000-0300-000013000000}"/>
+    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/top-view-of-a-binarytree/ojquestion" xr:uid="{00000000-0004-0000-0300-000014000000}"/>
+    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/diagonal-order-of-a-binarytree/ojquestion" xr:uid="{00000000-0004-0000-0300-000015000000}"/>
+    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/diagonal-order-(anti-clock-wise)-of-a-binarytree/ojquestion" xr:uid="{00000000-0004-0000-0300-000016000000}"/>
+    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/vertical-order-sum-of-a-binarytree/ojquestion" xr:uid="{00000000-0004-0000-0300-000017000000}"/>
+    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/diagonal-order-sum-of-a-binary-tree/ojquestion" xr:uid="{00000000-0004-0000-0300-000018000000}"/>
+    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/in-order-morris-traversal-in-binarytree/ojquestion" xr:uid="{00000000-0004-0000-0300-000019000000}"/>
+    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/pre-order-morris-traversal-in-binary-tree/ojquestion" xr:uid="{00000000-0004-0000-0300-00001A000000}"/>
+    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/bst-iterator/ojquestion" xr:uid="{00000000-0004-0000-0300-00001B000000}"/>
+    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/node-to-root-path-binary-tree/ojquestion" xr:uid="{00000000-0004-0000-0300-00001C000000}"/>
+    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/root-to-all-leaf-path-in-binary-tree/ojquestion" xr:uid="{00000000-0004-0000-0300-00001D000000}"/>
+    <hyperlink ref="B33" r:id="rId31" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/all-single-child-parent-in-binary-tree/ojquestion" xr:uid="{00000000-0004-0000-0300-00001E000000}"/>
+    <hyperlink ref="B34" r:id="rId32" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/trees/count-all-single-child-parent-in-binary-tree/ojquestion" xr:uid="{00000000-0004-0000-0300-00001F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A2:B50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4096,61 +4102,61 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/number-of-employees-under-every-manager-official/ojquestion"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/find-itinerary-from-tickets-official/ojquestion"/>
-    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/check-if-an-array-cab-be-divided-into-pairs-whose-sum-is-divisible-by-k-official/ojquestion"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/count-distinct-elements-in-every-window-of-size-k-official/ojquestion"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/largest-subarray-with-zero-sum-official/ojquestion"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/count-of-all-subarrays-with-zero-sum-official/ojquestion"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/largest-subarray-with-contiguous-elements-official/ojquestion"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/smallest-substring-of-a-string-containing-all-characters-of-another-string-official/ojquestion"/>
-    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/smallest-substring-of-a-string-containing-all-unique-characters-of-itself-official/ojquestion"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/longest-substring-with-unique-characters-official/ojquestion"/>
-    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/count-of-substrings-having-all-unique-characters-official/ojquestion"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/longest-substring-with-exactly-k-unique-characters-official/ojquestion"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/count-of-substrings-with-exactly-k-unique-characters-official/ojquestion"/>
-    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/equivalent-subarrays-official/ojquestion"/>
-    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/maximum-consecutive-ones-ii-official/ojquestion"/>
-    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/maximum-consecutive-ones-i-official/ojquestion"/>
-    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/longest-substring-with-at-most-k-unique-characters-official/ojquestion"/>
-    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/count-of-substrings-having-at-most-k-unique-characters-official/ojquestion"/>
-    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/binary-strings-with-substrings-representing-numbers-from-1-to-n-official/ojquestion"/>
-    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/count-of-subarrays-having-sum-equals-to-k-official/ojquestion"/>
-    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/find-all-anagrams-in-a-string-official/ojquestion"/>
-    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/k-anagrams-official/ojquestion"/>
-    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/find-anagram-mappings-official/ojquestion"/>
-    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/valid-anagram-official/ojquestion"/>
-    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/group-anagrams-official/ojquestion"/>
-    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/group-shifted-string-official/ojquestion"/>
-    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/isomorphic-strings-official/ojquestion"/>
-    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/word-pattern-official/ojquestion"/>
-    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/longest-subarray-with-sum-divisible-by-k-official/ojquestion"/>
-    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/count-of-subarrays-with-sum-divisible-by-k-official/ojquestion"/>
-    <hyperlink ref="B33" r:id="rId31" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/longest-subarray-with-equal-number-of-zeroes-and-ones-official/ojquestion"/>
-    <hyperlink ref="B34" r:id="rId32" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/count-of-subarrays-with-equal-number-of-zeroes-and-ones-official/ojquestion"/>
-    <hyperlink ref="B35" r:id="rId33" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/longest-subarray-with-equal-number-of-0s-1s-and-2s-official/ojquestion"/>
-    <hyperlink ref="B36" r:id="rId34" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/count-of-subarrays-with-equal-number-of-0s-1s-and-2s-official/ojquestion"/>
-    <hyperlink ref="B37" r:id="rId35" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/pairs-with-equal-sum-official/ojquestion"/>
-    <hyperlink ref="B38" r:id="rId36" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/recurring-sequence-in-a-fraction-official/ojquestion"/>
-    <hyperlink ref="B39" r:id="rId37" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/rabbits-in-the-forest-official/ojquestion"/>
-    <hyperlink ref="B40" r:id="rId38" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/double-pair-array-official/ojquestion"/>
-    <hyperlink ref="B41" r:id="rId39" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/maximum-points-on-a-line-official/ojquestion"/>
-    <hyperlink ref="B42" r:id="rId40" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/check-arithmetic-sequence-official/ojquestion"/>
-    <hyperlink ref="B43" r:id="rId41" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/smallest-subarray-with-all-occurrences-of-the-most-frequent-element-official/ojquestion"/>
-    <hyperlink ref="B44" r:id="rId42" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/task-completion-official/ojquestion"/>
-    <hyperlink ref="B45" r:id="rId43" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/pairs-with-given-sum-in-two-sorted-matrices-official/ojquestion"/>
-    <hyperlink ref="B46" r:id="rId44" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/quadruplet-sum-official/ojquestion"/>
-    <hyperlink ref="B47" r:id="rId45" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/quadruplet-sum-2-official/ojquestion"/>
-    <hyperlink ref="B48" r:id="rId46" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/powerful-number-official/ojquestion"/>
-    <hyperlink ref="B49" r:id="rId47" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/subdomain-visit-count-official/ojquestion"/>
-    <hyperlink ref="B50" r:id="rId48" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/first-non-repeating-character-official/ojquestion"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/number-of-employees-under-every-manager-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/find-itinerary-from-tickets-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/check-if-an-array-cab-be-divided-into-pairs-whose-sum-is-divisible-by-k-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/count-distinct-elements-in-every-window-of-size-k-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/largest-subarray-with-zero-sum-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/count-of-all-subarrays-with-zero-sum-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/largest-subarray-with-contiguous-elements-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/smallest-substring-of-a-string-containing-all-characters-of-another-string-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/smallest-substring-of-a-string-containing-all-unique-characters-of-itself-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000008000000}"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/longest-substring-with-unique-characters-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000009000000}"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/count-of-substrings-having-all-unique-characters-official/ojquestion" xr:uid="{00000000-0004-0000-0400-00000A000000}"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/longest-substring-with-exactly-k-unique-characters-official/ojquestion" xr:uid="{00000000-0004-0000-0400-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/count-of-substrings-with-exactly-k-unique-characters-official/ojquestion" xr:uid="{00000000-0004-0000-0400-00000C000000}"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/equivalent-subarrays-official/ojquestion" xr:uid="{00000000-0004-0000-0400-00000D000000}"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/maximum-consecutive-ones-ii-official/ojquestion" xr:uid="{00000000-0004-0000-0400-00000E000000}"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/maximum-consecutive-ones-i-official/ojquestion" xr:uid="{00000000-0004-0000-0400-00000F000000}"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/longest-substring-with-at-most-k-unique-characters-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000010000000}"/>
+    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/count-of-substrings-having-at-most-k-unique-characters-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000011000000}"/>
+    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/binary-strings-with-substrings-representing-numbers-from-1-to-n-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000012000000}"/>
+    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/count-of-subarrays-having-sum-equals-to-k-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000013000000}"/>
+    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/find-all-anagrams-in-a-string-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000014000000}"/>
+    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/k-anagrams-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000015000000}"/>
+    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/find-anagram-mappings-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000016000000}"/>
+    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/valid-anagram-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000017000000}"/>
+    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/group-anagrams-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000018000000}"/>
+    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/group-shifted-string-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000019000000}"/>
+    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/isomorphic-strings-official/ojquestion" xr:uid="{00000000-0004-0000-0400-00001A000000}"/>
+    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/word-pattern-official/ojquestion" xr:uid="{00000000-0004-0000-0400-00001B000000}"/>
+    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/longest-subarray-with-sum-divisible-by-k-official/ojquestion" xr:uid="{00000000-0004-0000-0400-00001C000000}"/>
+    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/count-of-subarrays-with-sum-divisible-by-k-official/ojquestion" xr:uid="{00000000-0004-0000-0400-00001D000000}"/>
+    <hyperlink ref="B33" r:id="rId31" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/longest-subarray-with-equal-number-of-zeroes-and-ones-official/ojquestion" xr:uid="{00000000-0004-0000-0400-00001E000000}"/>
+    <hyperlink ref="B34" r:id="rId32" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/count-of-subarrays-with-equal-number-of-zeroes-and-ones-official/ojquestion" xr:uid="{00000000-0004-0000-0400-00001F000000}"/>
+    <hyperlink ref="B35" r:id="rId33" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/longest-subarray-with-equal-number-of-0s-1s-and-2s-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000020000000}"/>
+    <hyperlink ref="B36" r:id="rId34" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/count-of-subarrays-with-equal-number-of-0s-1s-and-2s-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000021000000}"/>
+    <hyperlink ref="B37" r:id="rId35" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/pairs-with-equal-sum-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000022000000}"/>
+    <hyperlink ref="B38" r:id="rId36" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/recurring-sequence-in-a-fraction-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000023000000}"/>
+    <hyperlink ref="B39" r:id="rId37" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/rabbits-in-the-forest-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000024000000}"/>
+    <hyperlink ref="B40" r:id="rId38" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/double-pair-array-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000025000000}"/>
+    <hyperlink ref="B41" r:id="rId39" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/maximum-points-on-a-line-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000026000000}"/>
+    <hyperlink ref="B42" r:id="rId40" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/check-arithmetic-sequence-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000027000000}"/>
+    <hyperlink ref="B43" r:id="rId41" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/smallest-subarray-with-all-occurrences-of-the-most-frequent-element-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000028000000}"/>
+    <hyperlink ref="B44" r:id="rId42" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/task-completion-official/ojquestion" xr:uid="{00000000-0004-0000-0400-000029000000}"/>
+    <hyperlink ref="B45" r:id="rId43" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/pairs-with-given-sum-in-two-sorted-matrices-official/ojquestion" xr:uid="{00000000-0004-0000-0400-00002A000000}"/>
+    <hyperlink ref="B46" r:id="rId44" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/quadruplet-sum-official/ojquestion" xr:uid="{00000000-0004-0000-0400-00002B000000}"/>
+    <hyperlink ref="B47" r:id="rId45" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/quadruplet-sum-2-official/ojquestion" xr:uid="{00000000-0004-0000-0400-00002C000000}"/>
+    <hyperlink ref="B48" r:id="rId46" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/powerful-number-official/ojquestion" xr:uid="{00000000-0004-0000-0400-00002D000000}"/>
+    <hyperlink ref="B49" r:id="rId47" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/subdomain-visit-count-official/ojquestion" xr:uid="{00000000-0004-0000-0400-00002E000000}"/>
+    <hyperlink ref="B50" r:id="rId48" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/hashmap-and-heaps/first-non-repeating-character-official/ojquestion" xr:uid="{00000000-0004-0000-0400-00002F000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A2:B13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4260,24 +4266,24 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/bellman-ford-official/ojquestion"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/negative-weight-cycle-official/ojquestion"/>
-    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/pepcoder-and-reversing-official/ojquestion"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/pepcoding-course-schedule/ojquestion"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/kosaraju-algorithm-official/ojquestion"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/mother-vertex-official/ojquestion"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/minimum-cost-to-connect-all-cities-official/ojquestion"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/number-of-enclaves-official/ojquestion"/>
-    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/zero-one-matrix-official/ojquestion"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/number-of-distinct-island-official/ojquestion"/>
-    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/rotting-oranges-official/ojquestion"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/bellman-ford-official/ojquestion" xr:uid="{00000000-0004-0000-0500-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/negative-weight-cycle-official/ojquestion" xr:uid="{00000000-0004-0000-0500-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/pepcoder-and-reversing-official/ojquestion" xr:uid="{00000000-0004-0000-0500-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/pepcoding-course-schedule/ojquestion" xr:uid="{00000000-0004-0000-0500-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/kosaraju-algorithm-official/ojquestion" xr:uid="{00000000-0004-0000-0500-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/mother-vertex-official/ojquestion" xr:uid="{00000000-0004-0000-0500-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/minimum-cost-to-connect-all-cities-official/ojquestion" xr:uid="{00000000-0004-0000-0500-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/number-of-enclaves-official/ojquestion" xr:uid="{00000000-0004-0000-0500-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/zero-one-matrix-official/ojquestion" xr:uid="{00000000-0004-0000-0500-000008000000}"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/number-of-distinct-island-official/ojquestion" xr:uid="{00000000-0004-0000-0500-000009000000}"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/graphs/rotting-oranges-official/ojquestion" xr:uid="{00000000-0004-0000-0500-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A2:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4523,41 +4529,41 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/next-greater-element-i-official/ojquestion"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/next-greater-element-ii-official/ojquestion"/>
-    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/validate-stack-sequences-official/ojquestion"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/remove-outermost-parentheses-official/ojquestion"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/design-a-stack-with-increment-operation-official/ojquestion"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/minimum-add-to-make-parentheses-valid-official/ojquestion"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/score-of-parentheses-official/ojquestion"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/reverse-substrings-between-each-pair-of-parentheses-official/ojquestion"/>
-    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/minimum-remove-to-make-valid-parentheses-official/ojquestion"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/online-stock-span-official/ojquestion"/>
-    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/exclusive-time-of-functions-official/ojquestion"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/132-pattern-official/ojquestion"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/asteroid-collision-official/ojquestion"/>
-    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/remove-k-digits-official/ojquestion"/>
-    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/remove-duplicate-letters-official/ojquestion"/>
-    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/largest-area-histogram2-official/ojquestion"/>
-    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/maximal-rectangle-official/ojquestion"/>
-    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/trapping-rain-water-official/ojquestion"/>
-    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/number-of-valid-subarrays-official/ojquestion"/>
-    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/basic-calculator-official/ojquestion"/>
-    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/basic-calculator-ii-official/ojquestion"/>
-    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/basic-calculator-3-official/ojquestion"/>
-    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/lexicographically-smallest-subsequence-official/ojquestion"/>
-    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/design-circular-deque-official/ojquestion"/>
-    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/check-if-word-is-valid-after-insertion-official/ojquestion"/>
-    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/max-stack-offical/ojquestion"/>
-    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/number-of-recent-calls-official/ojquestion"/>
-    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/moving-average-from-data-stream-official/ojquestion"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/next-greater-element-i-official/ojquestion" xr:uid="{00000000-0004-0000-0600-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/next-greater-element-ii-official/ojquestion" xr:uid="{00000000-0004-0000-0600-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/validate-stack-sequences-official/ojquestion" xr:uid="{00000000-0004-0000-0600-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/remove-outermost-parentheses-official/ojquestion" xr:uid="{00000000-0004-0000-0600-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/design-a-stack-with-increment-operation-official/ojquestion" xr:uid="{00000000-0004-0000-0600-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/minimum-add-to-make-parentheses-valid-official/ojquestion" xr:uid="{00000000-0004-0000-0600-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/score-of-parentheses-official/ojquestion" xr:uid="{00000000-0004-0000-0600-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/reverse-substrings-between-each-pair-of-parentheses-official/ojquestion" xr:uid="{00000000-0004-0000-0600-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/minimum-remove-to-make-valid-parentheses-official/ojquestion" xr:uid="{00000000-0004-0000-0600-000008000000}"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/online-stock-span-official/ojquestion" xr:uid="{00000000-0004-0000-0600-000009000000}"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/exclusive-time-of-functions-official/ojquestion" xr:uid="{00000000-0004-0000-0600-00000A000000}"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/132-pattern-official/ojquestion" xr:uid="{00000000-0004-0000-0600-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/asteroid-collision-official/ojquestion" xr:uid="{00000000-0004-0000-0600-00000C000000}"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/remove-k-digits-official/ojquestion" xr:uid="{00000000-0004-0000-0600-00000D000000}"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/remove-duplicate-letters-official/ojquestion" xr:uid="{00000000-0004-0000-0600-00000E000000}"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/largest-area-histogram2-official/ojquestion" xr:uid="{00000000-0004-0000-0600-00000F000000}"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/maximal-rectangle-official/ojquestion" xr:uid="{00000000-0004-0000-0600-000010000000}"/>
+    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/trapping-rain-water-official/ojquestion" xr:uid="{00000000-0004-0000-0600-000011000000}"/>
+    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/number-of-valid-subarrays-official/ojquestion" xr:uid="{00000000-0004-0000-0600-000012000000}"/>
+    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/basic-calculator-official/ojquestion" xr:uid="{00000000-0004-0000-0600-000013000000}"/>
+    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/basic-calculator-ii-official/ojquestion" xr:uid="{00000000-0004-0000-0600-000014000000}"/>
+    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/basic-calculator-3-official/ojquestion" xr:uid="{00000000-0004-0000-0600-000015000000}"/>
+    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/lexicographically-smallest-subsequence-official/ojquestion" xr:uid="{00000000-0004-0000-0600-000016000000}"/>
+    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/design-circular-deque-official/ojquestion" xr:uid="{00000000-0004-0000-0600-000017000000}"/>
+    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/check-if-word-is-valid-after-insertion-official/ojquestion" xr:uid="{00000000-0004-0000-0600-000018000000}"/>
+    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/max-stack-offical/ojquestion" xr:uid="{00000000-0004-0000-0600-000019000000}"/>
+    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/number-of-recent-calls-official/ojquestion" xr:uid="{00000000-0004-0000-0600-00001A000000}"/>
+    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/stacks/moving-average-from-data-stream-official/ojquestion" xr:uid="{00000000-0004-0000-0600-00001B000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A2:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -4923,56 +4929,56 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/reverse-a-linkedlist/ojquestion"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/middle-of-a-linked-list/ojquestion"/>
-    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/palindrome-linkedlist-/ojquestion"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/fold-of-linkedlist/ojquestion"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/unfold-of-linkedlist/ojquestion"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/merge-two-sorted-linkedlist/ojquestion"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/merge-k-sorted-linkedlist/ojquestion"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/mergesort-linkedlist/ojquestion"/>
-    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/remove-nth-node-from-end-of-linkedlist/ojquestion"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/segregate-even-and-odd-nodes-in-a-link-list/ojquestion"/>
-    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/reverse-node-of-linkedlist-in-k-group/ojquestion"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/reverse-in-range/ojquestion"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/copy-linkedlist-with-random-pointers/ojquestion"/>
-    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/is-cycle-present-in-linkedlist/ojquestion"/>
-    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/cycle-node-in-linkedlist/ojquestion"/>
-    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/intersection-node-in-two-linkedlist-using-difference-method/ojquestion"/>
-    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/intersection-node-in-two-linkedlist-using-floyad-cycle-method/ojquestion"/>
-    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/add-two-linkedlist/ojquestion"/>
-    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/subtract-two-linkedlist/ojquestion"/>
-    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/multiply-two-linkedlist/ojquestion"/>
-    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/remove-duplicate-from-sorted-linkedlist/ojquestion"/>
-    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/remove-all-duplicates-from-sorted-linkedlist/ojquestion"/>
-    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/segregate-01-node-of-linkedlist-over-swapping-nodes/ojquestion"/>
-    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/segregate-01-node-of-linkedlist-by-swapping-data/ojquestion"/>
-    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/segregate-012-node-of-linkedlist-over-swapping-nodes/ojquestion"/>
-    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/segregate-012-node-of-linkedlist-by-swapping-data/ojquestion"/>
-    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/segregate-node-of-linkedlist-over-last-index./ojquestion"/>
-    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/segregate-node-of-linkedlist-over-pivot-index/ojquestion"/>
-    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/quicksort-in-linkedlist/ojquestion"/>
-    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/addfirst-in-doubly-linkedlist/ojquestion"/>
-    <hyperlink ref="B33" r:id="rId31" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/addlast-in-doubly-linkedlist/ojquestion"/>
-    <hyperlink ref="B34" r:id="rId32" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/remove-first-in-doubly-linkedlist/ojquestion"/>
-    <hyperlink ref="B35" r:id="rId33" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/remove-last-in-doubly-linkedlist/ojquestion"/>
-    <hyperlink ref="B36" r:id="rId34" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/get-first-and-get-last-in-doubly-linkedlist/ojquestion"/>
-    <hyperlink ref="B37" r:id="rId35" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/get-at-in-doubly-linkedlist/ojquestion"/>
-    <hyperlink ref="B38" r:id="rId36" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/add-at-in-doubly-linkedlist/ojquestion"/>
-    <hyperlink ref="B39" r:id="rId37" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/remove-at-in-doubly-linkedlist/ojquestion"/>
-    <hyperlink ref="B40" r:id="rId38" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/add-before-in-doubly-linkedlist/ojquestion"/>
-    <hyperlink ref="B41" r:id="rId39" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/add-after-in-doubly-linkedlist/ojquestion"/>
-    <hyperlink ref="B42" r:id="rId40" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/remove-after-in-doubly-linkedlist/ojquestion"/>
-    <hyperlink ref="B43" r:id="rId41" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/remove-before-in-doubly-linkedlist/ojquestion"/>
-    <hyperlink ref="B44" r:id="rId42" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/remove-node-in-doubly-linkedlist/ojquestion"/>
-    <hyperlink ref="B45" r:id="rId43" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/display-forward-and-backward-in-doubly-linkedlist/ojquestion"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/reverse-a-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/middle-of-a-linked-list/ojquestion" xr:uid="{00000000-0004-0000-0700-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/palindrome-linkedlist-/ojquestion" xr:uid="{00000000-0004-0000-0700-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/fold-of-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/unfold-of-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/merge-two-sorted-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/merge-k-sorted-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/mergesort-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/remove-nth-node-from-end-of-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000008000000}"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/segregate-even-and-odd-nodes-in-a-link-list/ojquestion" xr:uid="{00000000-0004-0000-0700-000009000000}"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/reverse-node-of-linkedlist-in-k-group/ojquestion" xr:uid="{00000000-0004-0000-0700-00000A000000}"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/reverse-in-range/ojquestion" xr:uid="{00000000-0004-0000-0700-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/copy-linkedlist-with-random-pointers/ojquestion" xr:uid="{00000000-0004-0000-0700-00000C000000}"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/is-cycle-present-in-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-00000D000000}"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/cycle-node-in-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-00000E000000}"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/intersection-node-in-two-linkedlist-using-difference-method/ojquestion" xr:uid="{00000000-0004-0000-0700-00000F000000}"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/intersection-node-in-two-linkedlist-using-floyad-cycle-method/ojquestion" xr:uid="{00000000-0004-0000-0700-000010000000}"/>
+    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/add-two-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000011000000}"/>
+    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/subtract-two-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000012000000}"/>
+    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/multiply-two-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000013000000}"/>
+    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/remove-duplicate-from-sorted-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000014000000}"/>
+    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/remove-all-duplicates-from-sorted-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000015000000}"/>
+    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/segregate-01-node-of-linkedlist-over-swapping-nodes/ojquestion" xr:uid="{00000000-0004-0000-0700-000016000000}"/>
+    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/segregate-01-node-of-linkedlist-by-swapping-data/ojquestion" xr:uid="{00000000-0004-0000-0700-000017000000}"/>
+    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/segregate-012-node-of-linkedlist-over-swapping-nodes/ojquestion" xr:uid="{00000000-0004-0000-0700-000018000000}"/>
+    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/segregate-012-node-of-linkedlist-by-swapping-data/ojquestion" xr:uid="{00000000-0004-0000-0700-000019000000}"/>
+    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/segregate-node-of-linkedlist-over-last-index./ojquestion" xr:uid="{00000000-0004-0000-0700-00001A000000}"/>
+    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/segregate-node-of-linkedlist-over-pivot-index/ojquestion" xr:uid="{00000000-0004-0000-0700-00001B000000}"/>
+    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/quicksort-in-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-00001C000000}"/>
+    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/addfirst-in-doubly-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-00001D000000}"/>
+    <hyperlink ref="B33" r:id="rId31" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/addlast-in-doubly-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-00001E000000}"/>
+    <hyperlink ref="B34" r:id="rId32" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/remove-first-in-doubly-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-00001F000000}"/>
+    <hyperlink ref="B35" r:id="rId33" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/remove-last-in-doubly-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000020000000}"/>
+    <hyperlink ref="B36" r:id="rId34" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/get-first-and-get-last-in-doubly-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000021000000}"/>
+    <hyperlink ref="B37" r:id="rId35" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/get-at-in-doubly-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000022000000}"/>
+    <hyperlink ref="B38" r:id="rId36" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/add-at-in-doubly-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000023000000}"/>
+    <hyperlink ref="B39" r:id="rId37" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/remove-at-in-doubly-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000024000000}"/>
+    <hyperlink ref="B40" r:id="rId38" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/add-before-in-doubly-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000025000000}"/>
+    <hyperlink ref="B41" r:id="rId39" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/add-after-in-doubly-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000026000000}"/>
+    <hyperlink ref="B42" r:id="rId40" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/remove-after-in-doubly-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000027000000}"/>
+    <hyperlink ref="B43" r:id="rId41" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/remove-before-in-doubly-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000028000000}"/>
+    <hyperlink ref="B44" r:id="rId42" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/remove-node-in-doubly-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-000029000000}"/>
+    <hyperlink ref="B45" r:id="rId43" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/linked-list/display-forward-and-backward-in-doubly-linkedlist/ojquestion" xr:uid="{00000000-0004-0000-0700-00002A000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A2:B42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5314,46 +5320,46 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/faulty_keyboard/ojquestion"/>
-    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/range_addition/ojquestion"/>
-    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/container_with_most_water/ojquestion"/>
-    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/squares-of-a-sorted-array/ojquestion"/>
-    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/majority-element-i/ojquestion"/>
-    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/majority-elements-ii/ojquestion"/>
-    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/majority-element-general/ojquestion"/>
-    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/next-greater-element-iii/ojquestion"/>
-    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/product-of-array-except-itself/ojquestion"/>
-    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/max-chunks-to-make-array-sorted/ojquestion"/>
-    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/max-chunks-to-make-array-sorted-2/ojquestion"/>
-    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/min_jumps_with_+i_-i_moves/ojquestion"/>
-    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/max-prod-of-three-nums/ojquestion"/>
-    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/sort_array_by_parity/ojquestion"/>
-    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/best-meeting-point/ojquestion"/>
-    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/sieve-of-eratosthenes/ojquestion"/>
-    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/transpose-matrix-mxn/ojquestion"/>
-    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/transpose-matrix-nxn/ojquestion"/>
-    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/rotate-image/ojquestion"/>
-    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/segmented-sieve/ojquestion"/>
-    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/reverse-vowels-of-a-string/ojquestion"/>
-    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/wiggle-sort-1/ojquestion"/>
-    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/multiply-strings/ojquestion"/>
-    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/pascals-triangle-2/ojquestion"/>
-    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/partition-labels/ojquestion"/>
-    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/minimum-number-of-platform/ojquestion"/>
-    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/valid-palindrome-2/ojquestion"/>
-    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/number-of-subarrays-with-bounded-maximum/ojquestion"/>
-    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/maximum-swap/ojquestion"/>
-    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/add-strings/ojquestion"/>
-    <hyperlink ref="B33" r:id="rId31" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/boats-to-save-people/ojquestion"/>
-    <hyperlink ref="B34" r:id="rId32" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/minimum-domino-rotations-for-equal-row/ojquestion"/>
-    <hyperlink ref="B35" r:id="rId33" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/merge_intervals_official/ojquestion"/>
-    <hyperlink ref="B36" r:id="rId34" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/meeting_rooms_one_official/ojquestion"/>
-    <hyperlink ref="B37" r:id="rId35" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/meeting_room_two_official/ojquestion"/>
-    <hyperlink ref="B38" r:id="rId36" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/interval_list_intersections_official/ojquestion"/>
-    <hyperlink ref="B39" r:id="rId37" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/insert_intervals_official/ojquestion"/>
-    <hyperlink ref="B40" r:id="rId38" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/find-minimum-number-of-arrows-needed-to-burst-balloon-official/ojquestion"/>
-    <hyperlink ref="B41" r:id="rId39" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/car-pooling-official/ojquestion"/>
-    <hyperlink ref="B42" r:id="rId40" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/min-len-of-string-after-removing-similar-ends-official/ojquestion"/>
+    <hyperlink ref="B3" r:id="rId1" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/faulty_keyboard/ojquestion" xr:uid="{00000000-0004-0000-0800-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/range_addition/ojquestion" xr:uid="{00000000-0004-0000-0800-000001000000}"/>
+    <hyperlink ref="B5" r:id="rId3" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/container_with_most_water/ojquestion" xr:uid="{00000000-0004-0000-0800-000002000000}"/>
+    <hyperlink ref="B6" r:id="rId4" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/squares-of-a-sorted-array/ojquestion" xr:uid="{00000000-0004-0000-0800-000003000000}"/>
+    <hyperlink ref="B7" r:id="rId5" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/majority-element-i/ojquestion" xr:uid="{00000000-0004-0000-0800-000004000000}"/>
+    <hyperlink ref="B8" r:id="rId6" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/majority-elements-ii/ojquestion" xr:uid="{00000000-0004-0000-0800-000005000000}"/>
+    <hyperlink ref="B9" r:id="rId7" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/majority-element-general/ojquestion" xr:uid="{00000000-0004-0000-0800-000006000000}"/>
+    <hyperlink ref="B10" r:id="rId8" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/next-greater-element-iii/ojquestion" xr:uid="{00000000-0004-0000-0800-000007000000}"/>
+    <hyperlink ref="B11" r:id="rId9" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/product-of-array-except-itself/ojquestion" xr:uid="{00000000-0004-0000-0800-000008000000}"/>
+    <hyperlink ref="B12" r:id="rId10" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/max-chunks-to-make-array-sorted/ojquestion" xr:uid="{00000000-0004-0000-0800-000009000000}"/>
+    <hyperlink ref="B13" r:id="rId11" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/max-chunks-to-make-array-sorted-2/ojquestion" xr:uid="{00000000-0004-0000-0800-00000A000000}"/>
+    <hyperlink ref="B14" r:id="rId12" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/min_jumps_with_+i_-i_moves/ojquestion" xr:uid="{00000000-0004-0000-0800-00000B000000}"/>
+    <hyperlink ref="B15" r:id="rId13" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/max-prod-of-three-nums/ojquestion" xr:uid="{00000000-0004-0000-0800-00000C000000}"/>
+    <hyperlink ref="B16" r:id="rId14" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/sort_array_by_parity/ojquestion" xr:uid="{00000000-0004-0000-0800-00000D000000}"/>
+    <hyperlink ref="B17" r:id="rId15" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/best-meeting-point/ojquestion" xr:uid="{00000000-0004-0000-0800-00000E000000}"/>
+    <hyperlink ref="B18" r:id="rId16" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/sieve-of-eratosthenes/ojquestion" xr:uid="{00000000-0004-0000-0800-00000F000000}"/>
+    <hyperlink ref="B19" r:id="rId17" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/transpose-matrix-mxn/ojquestion" xr:uid="{00000000-0004-0000-0800-000010000000}"/>
+    <hyperlink ref="B20" r:id="rId18" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/transpose-matrix-nxn/ojquestion" xr:uid="{00000000-0004-0000-0800-000011000000}"/>
+    <hyperlink ref="B21" r:id="rId19" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/rotate-image/ojquestion" xr:uid="{00000000-0004-0000-0800-000012000000}"/>
+    <hyperlink ref="B22" r:id="rId20" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/segmented-sieve/ojquestion" xr:uid="{00000000-0004-0000-0800-000013000000}"/>
+    <hyperlink ref="B23" r:id="rId21" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/reverse-vowels-of-a-string/ojquestion" xr:uid="{00000000-0004-0000-0800-000014000000}"/>
+    <hyperlink ref="B24" r:id="rId22" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/wiggle-sort-1/ojquestion" xr:uid="{00000000-0004-0000-0800-000015000000}"/>
+    <hyperlink ref="B25" r:id="rId23" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/multiply-strings/ojquestion" xr:uid="{00000000-0004-0000-0800-000016000000}"/>
+    <hyperlink ref="B26" r:id="rId24" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/pascals-triangle-2/ojquestion" xr:uid="{00000000-0004-0000-0800-000017000000}"/>
+    <hyperlink ref="B27" r:id="rId25" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/partition-labels/ojquestion" xr:uid="{00000000-0004-0000-0800-000018000000}"/>
+    <hyperlink ref="B28" r:id="rId26" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/minimum-number-of-platform/ojquestion" xr:uid="{00000000-0004-0000-0800-000019000000}"/>
+    <hyperlink ref="B29" r:id="rId27" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/valid-palindrome-2/ojquestion" xr:uid="{00000000-0004-0000-0800-00001A000000}"/>
+    <hyperlink ref="B30" r:id="rId28" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/number-of-subarrays-with-bounded-maximum/ojquestion" xr:uid="{00000000-0004-0000-0800-00001B000000}"/>
+    <hyperlink ref="B31" r:id="rId29" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/maximum-swap/ojquestion" xr:uid="{00000000-0004-0000-0800-00001C000000}"/>
+    <hyperlink ref="B32" r:id="rId30" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/add-strings/ojquestion" xr:uid="{00000000-0004-0000-0800-00001D000000}"/>
+    <hyperlink ref="B33" r:id="rId31" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/boats-to-save-people/ojquestion" xr:uid="{00000000-0004-0000-0800-00001E000000}"/>
+    <hyperlink ref="B34" r:id="rId32" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/minimum-domino-rotations-for-equal-row/ojquestion" xr:uid="{00000000-0004-0000-0800-00001F000000}"/>
+    <hyperlink ref="B35" r:id="rId33" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/merge_intervals_official/ojquestion" xr:uid="{00000000-0004-0000-0800-000020000000}"/>
+    <hyperlink ref="B36" r:id="rId34" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/meeting_rooms_one_official/ojquestion" xr:uid="{00000000-0004-0000-0800-000021000000}"/>
+    <hyperlink ref="B37" r:id="rId35" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/meeting_room_two_official/ojquestion" xr:uid="{00000000-0004-0000-0800-000022000000}"/>
+    <hyperlink ref="B38" r:id="rId36" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/interval_list_intersections_official/ojquestion" xr:uid="{00000000-0004-0000-0800-000023000000}"/>
+    <hyperlink ref="B39" r:id="rId37" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/insert_intervals_official/ojquestion" xr:uid="{00000000-0004-0000-0800-000024000000}"/>
+    <hyperlink ref="B40" r:id="rId38" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/find-minimum-number-of-arrows-needed-to-burst-balloon-official/ojquestion" xr:uid="{00000000-0004-0000-0800-000025000000}"/>
+    <hyperlink ref="B41" r:id="rId39" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/car-pooling-official/ojquestion" xr:uid="{00000000-0004-0000-0800-000026000000}"/>
+    <hyperlink ref="B42" r:id="rId40" display="https://www.pepcoding.com/resources/data-structures-and-algorithms-in-java-levelup/arrays-and-strings/min-len-of-string-after-removing-similar-ends-official/ojquestion" xr:uid="{00000000-0004-0000-0800-000027000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>